<commit_message>
update code review and documentation about requirement refinement.
</commit_message>
<xml_diff>
--- a/bts_effort_여기다업데이트해주세요.xlsx
+++ b/bts_effort_여기다업데이트해주세요.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shchin/sdet/CMU/project/presentation/share_doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SDET_CODE\share_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30057839-8AAA-B74B-9692-49551BC0D7CF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="3" r:id="rId1"/>
@@ -18,9 +17,6 @@
     <sheet name="AC" sheetId="9" r:id="rId3"/>
     <sheet name="©" sheetId="11" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
     <definedName name="holidays">OFFSET(#REF!,1,0,COUNTA(#REF!),1)</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">AC!$A$2:$O$3</definedName>
@@ -31,17 +27,17 @@
     <definedName name="vertex42_id" hidden="1">"earned-value-management.xlsx"</definedName>
     <definedName name="vertex42_title" hidden="1">"Earned Value Management Template"</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Vertex42</author>
   </authors>
   <commentList>
-    <comment ref="A21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="C21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -261,7 +257,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
@@ -1214,7 +1210,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ko-KR"/>
   <c:roundedCorners val="0"/>
@@ -1281,79 +1277,79 @@
                   <c:v>in Korea</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.9</c:v>
+                  <c:v>07-09</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.10</c:v>
+                  <c:v>07-10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.11</c:v>
+                  <c:v>07-11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.12</c:v>
+                  <c:v>07-12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.13</c:v>
+                  <c:v>07-13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.14</c:v>
+                  <c:v>07-14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.15</c:v>
+                  <c:v>07-15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.16</c:v>
+                  <c:v>07-16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.17</c:v>
+                  <c:v>07-17</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.18</c:v>
+                  <c:v>07-18</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.19</c:v>
+                  <c:v>07-19</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.20</c:v>
+                  <c:v>07-20</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.21</c:v>
+                  <c:v>07-21</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.22</c:v>
+                  <c:v>07-22</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.23</c:v>
+                  <c:v>07-23</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.24</c:v>
+                  <c:v>07-24</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.25</c:v>
+                  <c:v>07-25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.26</c:v>
+                  <c:v>07-26</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.27</c:v>
+                  <c:v>07-27</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.28</c:v>
+                  <c:v>07-28</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.29</c:v>
+                  <c:v>07-29</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.30</c:v>
+                  <c:v>07-30</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.31</c:v>
+                  <c:v>07-31</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.1</c:v>
+                  <c:v>08-01</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.2</c:v>
+                  <c:v>08-02</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1410,43 +1406,43 @@
                   <c:v>205</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>230</c:v>
+                  <c:v>235</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>250</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>270</c:v>
+                  <c:v>285</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>295</c:v>
+                  <c:v>310</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>320</c:v>
+                  <c:v>335</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>320</c:v>
+                  <c:v>335</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>320</c:v>
+                  <c:v>335</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>350</c:v>
+                  <c:v>365</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>380</c:v>
+                  <c:v>395</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>400</c:v>
+                  <c:v>415</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>420</c:v>
+                  <c:v>435</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0B77-4BB5-85C2-863F16D3AB54}"/>
             </c:ext>
@@ -1490,79 +1486,79 @@
                   <c:v>in Korea</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.9</c:v>
+                  <c:v>07-09</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.10</c:v>
+                  <c:v>07-10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.11</c:v>
+                  <c:v>07-11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.12</c:v>
+                  <c:v>07-12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.13</c:v>
+                  <c:v>07-13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.14</c:v>
+                  <c:v>07-14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.15</c:v>
+                  <c:v>07-15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.16</c:v>
+                  <c:v>07-16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.17</c:v>
+                  <c:v>07-17</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.18</c:v>
+                  <c:v>07-18</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.19</c:v>
+                  <c:v>07-19</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.20</c:v>
+                  <c:v>07-20</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.21</c:v>
+                  <c:v>07-21</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.22</c:v>
+                  <c:v>07-22</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.23</c:v>
+                  <c:v>07-23</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.24</c:v>
+                  <c:v>07-24</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.25</c:v>
+                  <c:v>07-25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.26</c:v>
+                  <c:v>07-26</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.27</c:v>
+                  <c:v>07-27</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.28</c:v>
+                  <c:v>07-28</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.29</c:v>
+                  <c:v>07-29</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.30</c:v>
+                  <c:v>07-30</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.31</c:v>
+                  <c:v>07-31</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.1</c:v>
+                  <c:v>08-01</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.2</c:v>
+                  <c:v>08-02</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1655,7 +1651,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0B77-4BB5-85C2-863F16D3AB54}"/>
             </c:ext>
@@ -1699,79 +1695,79 @@
                   <c:v>in Korea</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.9</c:v>
+                  <c:v>07-09</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.10</c:v>
+                  <c:v>07-10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.11</c:v>
+                  <c:v>07-11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.12</c:v>
+                  <c:v>07-12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.13</c:v>
+                  <c:v>07-13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.14</c:v>
+                  <c:v>07-14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.15</c:v>
+                  <c:v>07-15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.16</c:v>
+                  <c:v>07-16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.17</c:v>
+                  <c:v>07-17</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.18</c:v>
+                  <c:v>07-18</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.19</c:v>
+                  <c:v>07-19</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.20</c:v>
+                  <c:v>07-20</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.21</c:v>
+                  <c:v>07-21</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.22</c:v>
+                  <c:v>07-22</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.23</c:v>
+                  <c:v>07-23</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.24</c:v>
+                  <c:v>07-24</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.25</c:v>
+                  <c:v>07-25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.26</c:v>
+                  <c:v>07-26</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.27</c:v>
+                  <c:v>07-27</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.28</c:v>
+                  <c:v>07-28</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.29</c:v>
+                  <c:v>07-29</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.30</c:v>
+                  <c:v>07-30</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.31</c:v>
+                  <c:v>07-31</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.1</c:v>
+                  <c:v>08-01</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.2</c:v>
+                  <c:v>08-02</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1864,7 +1860,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0B77-4BB5-85C2-863F16D3AB54}"/>
             </c:ext>
@@ -1880,11 +1876,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="188275328"/>
-        <c:axId val="190614912"/>
+        <c:axId val="146881552"/>
+        <c:axId val="146912560"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="188275328"/>
+        <c:axId val="146881552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1958,7 +1954,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190614912"/>
+        <c:crossAx val="146912560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -1967,7 +1963,7 @@
         <c:minorUnit val="1"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="190614912"/>
+        <c:axId val="146912560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1990,6 +1986,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0_);[Red]\(#,##0\)" sourceLinked="0"/>
@@ -2021,7 +2018,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188275328"/>
+        <c:crossAx val="146881552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2131,7 +2128,7 @@
         <xdr:cNvPr id="1063" name="Chart 39">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000027040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2170,7 +2167,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2220,7 +2217,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2270,7 +2267,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2320,7 +2317,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2347,19 +2344,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Report"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2624,26 +2608,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AC47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I16" zoomScale="150" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" customWidth="1"/>
-    <col min="4" max="15" width="8.6640625" customWidth="1"/>
-    <col min="17" max="17" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
+    <col min="4" max="15" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20">
+    <row r="1" spans="1:17" ht="20.25">
       <c r="A1" s="17" t="s">
         <v>3</v>
       </c>
@@ -2656,7 +2640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16">
+    <row r="2" spans="1:17" ht="15.75">
       <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
@@ -2844,7 +2828,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:29" ht="16">
+    <row r="20" spans="1:29" ht="15.75">
       <c r="A20" s="11" t="s">
         <v>31</v>
       </c>
@@ -2992,7 +2976,7 @@
       </c>
       <c r="C23" s="23">
         <f t="shared" ref="C23:C33" si="0">SUM(D23:AC23)</f>
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D23" s="30"/>
       <c r="E23" s="30">
@@ -3019,9 +3003,15 @@
       <c r="P23" s="30"/>
       <c r="Q23" s="30"/>
       <c r="R23" s="30"/>
-      <c r="S23" s="30"/>
-      <c r="T23" s="30"/>
-      <c r="U23" s="30"/>
+      <c r="S23" s="30">
+        <v>3</v>
+      </c>
+      <c r="T23" s="30">
+        <v>3</v>
+      </c>
+      <c r="U23" s="30">
+        <v>3</v>
+      </c>
       <c r="V23" s="30"/>
       <c r="W23" s="30"/>
       <c r="X23" s="30"/>
@@ -3288,7 +3278,7 @@
       </c>
       <c r="C29" s="23">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D29" s="30"/>
       <c r="E29" s="30"/>
@@ -3305,9 +3295,15 @@
       <c r="P29" s="30"/>
       <c r="Q29" s="30"/>
       <c r="R29" s="30"/>
-      <c r="S29" s="30"/>
-      <c r="T29" s="30"/>
-      <c r="U29" s="30"/>
+      <c r="S29" s="30">
+        <v>2</v>
+      </c>
+      <c r="T29" s="30">
+        <v>2</v>
+      </c>
+      <c r="U29" s="30">
+        <v>2</v>
+      </c>
       <c r="V29" s="30"/>
       <c r="W29" s="30"/>
       <c r="X29" s="30"/>
@@ -3499,7 +3495,7 @@
       </c>
       <c r="C35" s="25">
         <f>SUM(C22:C33)</f>
-        <v>420</v>
+        <v>435</v>
       </c>
       <c r="D35" s="27">
         <f>SUM(D22:D34)</f>
@@ -3563,15 +3559,15 @@
       </c>
       <c r="S35" s="27">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="T35" s="27">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="U35" s="27">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="V35" s="27">
         <f t="shared" si="3"/>
@@ -3674,47 +3670,47 @@
       </c>
       <c r="S36" s="29">
         <f>IF(ISBLANK(S21),NA(),SUM($D35:S35))</f>
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="T36" s="29">
         <f>IF(ISBLANK(T21),NA(),SUM($D35:T35))</f>
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="U36" s="29">
         <f>IF(ISBLANK(U21),NA(),SUM($D35:U35))</f>
-        <v>270</v>
+        <v>285</v>
       </c>
       <c r="V36" s="29">
         <f>IF(ISBLANK(V21),NA(),SUM($D35:V35))</f>
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="W36" s="29">
         <f>IF(ISBLANK(W21),NA(),SUM($D35:W35))</f>
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="X36" s="29">
         <f>IF(ISBLANK(X21),NA(),SUM($D35:X35))</f>
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="Y36" s="29">
         <f>IF(ISBLANK(Y21),NA(),SUM($D35:Y35))</f>
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="Z36" s="29">
         <f>IF(ISBLANK(Z21),NA(),SUM($D35:Z35))</f>
-        <v>350</v>
+        <v>365</v>
       </c>
       <c r="AA36" s="29">
         <f>IF(ISBLANK(AA21),NA(),SUM($D35:AA35))</f>
-        <v>380</v>
+        <v>395</v>
       </c>
       <c r="AB36" s="29">
         <f>IF(ISBLANK(AB21),NA(),SUM($D35:AB35))</f>
-        <v>400</v>
+        <v>415</v>
       </c>
       <c r="AC36" s="29">
         <f>IF(ISBLANK(AC21),NA(),SUM($D35:AC35))</f>
-        <v>420</v>
+        <v>435</v>
       </c>
     </row>
     <row r="37" spans="1:29">
@@ -3748,7 +3744,7 @@
       <c r="AB37" s="24"/>
       <c r="AC37" s="24"/>
     </row>
-    <row r="38" spans="1:29" ht="16">
+    <row r="38" spans="1:29" ht="15.75">
       <c r="A38" s="3" t="s">
         <v>38</v>
       </c>
@@ -4006,7 +4002,7 @@
       <c r="AB41" s="24"/>
       <c r="AC41" s="24"/>
     </row>
-    <row r="42" spans="1:29" ht="16">
+    <row r="42" spans="1:29" ht="15.75">
       <c r="A42" s="3" t="s">
         <v>20</v>
       </c>
@@ -4186,47 +4182,47 @@
       </c>
       <c r="S44" s="10">
         <f t="shared" si="9"/>
-        <v>-38.300000000000011</v>
+        <v>-43.300000000000011</v>
       </c>
       <c r="T44" s="10">
         <f t="shared" si="9"/>
-        <v>-43.300000000000011</v>
+        <v>-53.300000000000011</v>
       </c>
       <c r="U44" s="10">
         <f t="shared" si="9"/>
-        <v>-30.300000000000011</v>
+        <v>-45.300000000000011</v>
       </c>
       <c r="V44" s="10">
         <f t="shared" si="9"/>
-        <v>-30.300000000000011</v>
+        <v>-45.300000000000011</v>
       </c>
       <c r="W44" s="10">
         <f t="shared" si="9"/>
-        <v>-44.300000000000011</v>
+        <v>-59.300000000000011</v>
       </c>
       <c r="X44" s="10">
         <f t="shared" si="9"/>
-        <v>-34.300000000000011</v>
+        <v>-49.300000000000011</v>
       </c>
       <c r="Y44" s="10">
         <f t="shared" si="9"/>
-        <v>-24.300000000000011</v>
+        <v>-39.300000000000011</v>
       </c>
       <c r="Z44" s="10">
         <f t="shared" si="9"/>
-        <v>-18.300000000000011</v>
+        <v>-33.300000000000011</v>
       </c>
       <c r="AA44" s="10">
         <f t="shared" si="9"/>
-        <v>-29.800000000000011</v>
+        <v>-44.800000000000011</v>
       </c>
       <c r="AB44" s="10">
         <f t="shared" si="9"/>
-        <v>-49.800000000000011</v>
+        <v>-64.800000000000011</v>
       </c>
       <c r="AC44" s="10">
         <f t="shared" si="9"/>
-        <v>-69.800000000000011</v>
+        <v>-84.800000000000011</v>
       </c>
     </row>
     <row r="45" spans="1:29">
@@ -4404,47 +4400,47 @@
       </c>
       <c r="S46" s="35">
         <f t="shared" si="15"/>
-        <v>0.83347826086956511</v>
+        <v>0.81574468085106377</v>
       </c>
       <c r="T46" s="35">
         <f t="shared" si="15"/>
-        <v>0.82679999999999998</v>
+        <v>0.79499999999999993</v>
       </c>
       <c r="U46" s="35">
         <f t="shared" si="15"/>
-        <v>0.88777777777777778</v>
+        <v>0.84105263157894727</v>
       </c>
       <c r="V46" s="35">
         <f t="shared" si="15"/>
-        <v>0.89728813559322029</v>
+        <v>0.85387096774193549</v>
       </c>
       <c r="W46" s="35">
         <f t="shared" si="15"/>
-        <v>0.86156250000000001</v>
+        <v>0.82298507462686565</v>
       </c>
       <c r="X46" s="35">
         <f t="shared" si="15"/>
-        <v>0.89281250000000001</v>
+        <v>0.85283582089552235</v>
       </c>
       <c r="Y46" s="35">
         <f t="shared" si="15"/>
-        <v>0.92406250000000001</v>
+        <v>0.88268656716417904</v>
       </c>
       <c r="Z46" s="35">
         <f t="shared" si="15"/>
-        <v>0.94771428571428573</v>
+        <v>0.90876712328767117</v>
       </c>
       <c r="AA46" s="35">
         <f t="shared" si="15"/>
-        <v>0.92157894736842105</v>
+        <v>0.88658227848101268</v>
       </c>
       <c r="AB46" s="35">
         <f t="shared" si="15"/>
-        <v>0.87549999999999994</v>
+        <v>0.84385542168674699</v>
       </c>
       <c r="AC46" s="35">
         <f t="shared" si="15"/>
-        <v>0.83380952380952378</v>
+        <v>0.80505747126436777</v>
       </c>
     </row>
     <row r="47" spans="1:29">
@@ -4453,107 +4449,107 @@
       </c>
       <c r="D47" s="36">
         <f>IF(AND(ISBLANK(D39),ISBLANK(D40))," - ",$C$35/D45)</f>
-        <v>306.60000000000002</v>
+        <v>317.55</v>
       </c>
       <c r="E47" s="36">
         <f t="shared" ref="E47:O47" si="16">IF(AND(ISBLANK(E39),ISBLANK(E40))," - ",$C$35/E45)</f>
-        <v>320.94339622641508</v>
+        <v>332.40566037735846</v>
       </c>
       <c r="F47" s="36">
         <f t="shared" si="16"/>
-        <v>327.89473684210526</v>
+        <v>339.60526315789474</v>
       </c>
       <c r="G47" s="36">
         <f t="shared" si="16"/>
-        <v>335.32258064516128</v>
+        <v>347.29838709677415</v>
       </c>
       <c r="H47" s="36">
         <f t="shared" si="16"/>
-        <v>341.64179104477614</v>
+        <v>353.84328358208955</v>
       </c>
       <c r="I47" s="36">
         <f t="shared" si="16"/>
-        <v>350.30303030303031</v>
+        <v>362.8138528138528</v>
       </c>
       <c r="J47" s="36">
         <f t="shared" si="16"/>
-        <v>350.30303030303031</v>
+        <v>362.8138528138528</v>
       </c>
       <c r="K47" s="36">
         <f t="shared" si="16"/>
-        <v>350.9012875536481</v>
+        <v>363.43347639484978</v>
       </c>
       <c r="L47" s="36">
         <f t="shared" si="16"/>
-        <v>371.32450331125824</v>
+        <v>384.58609271523176</v>
       </c>
       <c r="M47" s="36">
         <f t="shared" si="16"/>
-        <v>403.59374999999994</v>
+        <v>418.00781249999994</v>
       </c>
       <c r="N47" s="36">
         <f t="shared" si="16"/>
-        <v>392.33009708737865</v>
+        <v>406.34188626907076</v>
       </c>
       <c r="O47" s="36">
         <f t="shared" si="16"/>
-        <v>392.33009708737865</v>
+        <v>406.34188626907076</v>
       </c>
       <c r="P47" s="36">
         <f t="shared" ref="P47:Q47" si="17">IF(AND(ISBLANK(P39),ISBLANK(P40))," - ",$C$35/P45)</f>
-        <v>388.50629874025196</v>
+        <v>402.38152369526097</v>
       </c>
       <c r="Q47" s="36">
         <f t="shared" si="17"/>
-        <v>388.50629874025196</v>
+        <v>402.38152369526097</v>
       </c>
       <c r="R47" s="36">
         <f t="shared" ref="R47:AC47" si="18">IF(AND(ISBLANK(R39),ISBLANK(R40))," - ",$C$35/R45)</f>
-        <v>437.33626857457347</v>
+        <v>452.95542102366534</v>
       </c>
       <c r="S47" s="36">
         <f t="shared" si="18"/>
-        <v>438.62284820031294</v>
+        <v>454.28794992175273</v>
       </c>
       <c r="T47" s="36">
         <f t="shared" si="18"/>
-        <v>427.11175616835993</v>
+        <v>442.36574746008711</v>
       </c>
       <c r="U47" s="36">
         <f t="shared" si="18"/>
-        <v>409.31163954943685</v>
+        <v>423.92991239048814</v>
       </c>
       <c r="V47" s="36">
         <f t="shared" si="18"/>
-        <v>402.38760861352472</v>
+        <v>416.75859463543634</v>
       </c>
       <c r="W47" s="36">
         <f t="shared" si="18"/>
-        <v>404.30903155603914</v>
+        <v>418.74863982589767</v>
       </c>
       <c r="X47" s="36">
         <f t="shared" si="18"/>
-        <v>412.2086104305215</v>
+        <v>426.93034651732586</v>
       </c>
       <c r="Y47" s="36">
         <f t="shared" si="18"/>
-        <v>419.57389245857286</v>
+        <v>434.55867433209335</v>
       </c>
       <c r="Z47" s="36">
         <f t="shared" si="18"/>
-        <v>412.02291227012358</v>
+        <v>426.73801627977087</v>
       </c>
       <c r="AA47" s="36">
         <f t="shared" si="18"/>
-        <v>409.44603083952023</v>
+        <v>424.06910336950313</v>
       </c>
       <c r="AB47" s="36">
         <f t="shared" si="18"/>
-        <v>409.44603083952023</v>
+        <v>424.06910336950313</v>
       </c>
       <c r="AC47" s="36">
         <f t="shared" si="18"/>
-        <v>409.44603083952023</v>
+        <v>424.06910336950313</v>
       </c>
     </row>
   </sheetData>
@@ -4580,7 +4576,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="Q3" r:id="rId1" display="https://www.vertex42.com/ExcelTemplates/earned-value-management.html" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="Q3" r:id="rId1" display="https://www.vertex42.com/ExcelTemplates/earned-value-management.html"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.25" bottom="0.5" header="0.5" footer="0.25"/>
   <pageSetup scale="91" orientation="landscape" r:id="rId2"/>
@@ -4593,7 +4589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -4603,21 +4599,21 @@
       <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="6.5" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="6.5" customWidth="1"/>
-    <col min="4" max="15" width="8.6640625" customWidth="1"/>
-    <col min="17" max="17" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="15" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="20">
+    <row r="1" spans="1:29" ht="20.25">
       <c r="A1" s="22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="16">
+    <row r="2" spans="1:29" ht="15.75">
       <c r="A2" s="11"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4812,7 +4808,7 @@
       </c>
       <c r="C10">
         <f>Report!C23</f>
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D10" s="68"/>
       <c r="E10" s="68">
@@ -5116,7 +5112,7 @@
       </c>
       <c r="C16">
         <f>Report!C29</f>
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D16" s="68"/>
       <c r="E16" s="68"/>
@@ -5570,23 +5566,23 @@
       </c>
       <c r="E24" s="21">
         <f t="shared" ref="E24:AC24" si="1">SUMPRODUCT(E9:E21,$C$9:$C$21)</f>
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="F24" s="21">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>236</v>
       </c>
       <c r="G24" s="21">
         <f t="shared" si="1"/>
-        <v>250</v>
+        <v>295</v>
       </c>
       <c r="H24" s="21">
         <f t="shared" si="1"/>
-        <v>250</v>
+        <v>295</v>
       </c>
       <c r="I24" s="21">
         <f t="shared" si="1"/>
-        <v>114.99999999999999</v>
+        <v>135.69999999999999</v>
       </c>
       <c r="J24" s="21">
         <f t="shared" si="1"/>
@@ -5594,19 +5590,19 @@
       </c>
       <c r="K24" s="21">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>35.4</v>
       </c>
       <c r="L24" s="21">
         <f t="shared" si="1"/>
-        <v>1170</v>
+        <v>1203.3</v>
       </c>
       <c r="M24" s="21">
         <f t="shared" si="1"/>
-        <v>1365</v>
+        <v>1433.4</v>
       </c>
       <c r="N24" s="21">
         <f t="shared" si="1"/>
-        <v>1585</v>
+        <v>1603</v>
       </c>
       <c r="O24" s="21">
         <f t="shared" si="1"/>
@@ -5614,7 +5610,7 @@
       </c>
       <c r="P24" s="21">
         <f t="shared" si="1"/>
-        <v>1350</v>
+        <v>1368</v>
       </c>
       <c r="Q24" s="21">
         <f t="shared" si="1"/>
@@ -5622,7 +5618,7 @@
       </c>
       <c r="R24" s="21">
         <f t="shared" si="1"/>
-        <v>900</v>
+        <v>990</v>
       </c>
       <c r="S24" s="21">
         <f t="shared" si="1"/>
@@ -5658,7 +5654,7 @@
       </c>
       <c r="AA24" s="21">
         <f t="shared" si="1"/>
-        <v>1120</v>
+        <v>1210</v>
       </c>
       <c r="AB24" s="21">
         <f t="shared" si="1"/>
@@ -5672,7 +5668,7 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Q3" r:id="rId1" display="https://www.vertex42.com/ExcelTemplates/earned-value-management.html" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="Q3" r:id="rId1" display="https://www.vertex42.com/ExcelTemplates/earned-value-management.html"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.25" bottom="0.25" header="0.5" footer="0.25"/>
   <pageSetup scale="93" orientation="landscape" r:id="rId2"/>
@@ -5682,7 +5678,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5692,21 +5688,21 @@
       <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="6.5" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="6.5" customWidth="1"/>
-    <col min="4" max="15" width="8.6640625" customWidth="1"/>
-    <col min="17" max="17" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="15" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="20">
+    <row r="1" spans="1:29" ht="20.25">
       <c r="A1" s="22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="16">
+    <row r="2" spans="1:29" ht="15.75">
       <c r="A2" s="11"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -6604,7 +6600,7 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Q3" r:id="rId1" display="https://www.vertex42.com/ExcelTemplates/earned-value-management.html" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="Q3" r:id="rId1" display="https://www.vertex42.com/ExcelTemplates/earned-value-management.html"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.25" bottom="0.25" header="0.5" footer="0.25"/>
   <pageSetup scale="93" orientation="landscape" r:id="rId2"/>
@@ -6614,19 +6610,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="5.5" customWidth="1"/>
-    <col min="2" max="2" width="78.5" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="78.42578125" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1">
@@ -6637,12 +6633,12 @@
       <c r="C1" s="37"/>
       <c r="D1" s="29"/>
     </row>
-    <row r="2" spans="1:4" ht="14">
+    <row r="2" spans="1:4" ht="16.5">
       <c r="A2" s="38"/>
       <c r="B2" s="39"/>
       <c r="C2" s="38"/>
     </row>
-    <row r="3" spans="1:4" s="42" customFormat="1" ht="14">
+    <row r="3" spans="1:4" s="42" customFormat="1" ht="14.25">
       <c r="A3" s="40"/>
       <c r="B3" s="41" t="s">
         <v>39</v>
@@ -6656,109 +6652,109 @@
       </c>
       <c r="C4" s="40"/>
     </row>
-    <row r="5" spans="1:4" s="42" customFormat="1" ht="16">
+    <row r="5" spans="1:4" s="42" customFormat="1" ht="15">
       <c r="A5" s="40"/>
       <c r="B5" s="44"/>
       <c r="C5" s="40"/>
     </row>
-    <row r="6" spans="1:4" s="42" customFormat="1" ht="16">
+    <row r="6" spans="1:4" s="42" customFormat="1" ht="15.75">
       <c r="A6" s="40"/>
       <c r="B6" s="45" t="s">
         <v>46</v>
       </c>
       <c r="C6" s="40"/>
     </row>
-    <row r="7" spans="1:4" s="42" customFormat="1" ht="16">
+    <row r="7" spans="1:4" s="42" customFormat="1" ht="15.75">
       <c r="A7" s="46"/>
       <c r="B7" s="44"/>
       <c r="C7" s="47"/>
     </row>
-    <row r="8" spans="1:4" s="42" customFormat="1" ht="32">
+    <row r="8" spans="1:4" s="42" customFormat="1" ht="30">
       <c r="A8" s="48"/>
       <c r="B8" s="44" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="40"/>
     </row>
-    <row r="9" spans="1:4" s="42" customFormat="1" ht="16">
+    <row r="9" spans="1:4" s="42" customFormat="1" ht="15">
       <c r="A9" s="48"/>
       <c r="B9" s="44"/>
       <c r="C9" s="40"/>
     </row>
-    <row r="10" spans="1:4" s="42" customFormat="1" ht="32">
+    <row r="10" spans="1:4" s="42" customFormat="1" ht="30">
       <c r="A10" s="48"/>
       <c r="B10" s="44" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="40"/>
     </row>
-    <row r="11" spans="1:4" s="42" customFormat="1" ht="16">
+    <row r="11" spans="1:4" s="42" customFormat="1" ht="15">
       <c r="A11" s="48"/>
       <c r="B11" s="44"/>
       <c r="C11" s="40"/>
     </row>
-    <row r="12" spans="1:4" s="42" customFormat="1" ht="32">
+    <row r="12" spans="1:4" s="42" customFormat="1" ht="30">
       <c r="A12" s="48"/>
       <c r="B12" s="44" t="s">
         <v>42</v>
       </c>
       <c r="C12" s="40"/>
     </row>
-    <row r="13" spans="1:4" s="42" customFormat="1" ht="16">
+    <row r="13" spans="1:4" s="42" customFormat="1" ht="15">
       <c r="A13" s="48"/>
       <c r="B13" s="44"/>
       <c r="C13" s="40"/>
     </row>
-    <row r="14" spans="1:4" s="42" customFormat="1" ht="16">
+    <row r="14" spans="1:4" s="42" customFormat="1" ht="15">
       <c r="A14" s="48"/>
       <c r="B14" s="63" t="s">
         <v>45</v>
       </c>
       <c r="C14" s="40"/>
     </row>
-    <row r="15" spans="1:4" s="42" customFormat="1" ht="16">
+    <row r="15" spans="1:4" s="42" customFormat="1" ht="15">
       <c r="A15" s="48"/>
       <c r="B15" s="44"/>
       <c r="C15" s="40"/>
     </row>
-    <row r="16" spans="1:4" s="42" customFormat="1" ht="16">
+    <row r="16" spans="1:4" s="42" customFormat="1" ht="15.75">
       <c r="A16" s="48"/>
       <c r="B16" s="62" t="s">
         <v>47</v>
       </c>
       <c r="C16" s="40"/>
     </row>
-    <row r="17" spans="1:3" s="42" customFormat="1" ht="14">
+    <row r="17" spans="1:3" s="42" customFormat="1" ht="16.5">
       <c r="A17" s="48"/>
       <c r="B17" s="49"/>
       <c r="C17" s="40"/>
     </row>
-    <row r="18" spans="1:3" s="42" customFormat="1" ht="14">
+    <row r="18" spans="1:3" s="42" customFormat="1" ht="16.5">
       <c r="A18" s="48"/>
       <c r="B18" s="49"/>
       <c r="C18" s="40"/>
     </row>
-    <row r="19" spans="1:3" s="42" customFormat="1" ht="14">
+    <row r="19" spans="1:3" s="42" customFormat="1" ht="14.25">
       <c r="A19" s="48"/>
       <c r="B19" s="50"/>
       <c r="C19" s="40"/>
     </row>
-    <row r="20" spans="1:3" s="42" customFormat="1" ht="14">
+    <row r="20" spans="1:3" s="42" customFormat="1" ht="15">
       <c r="A20" s="46"/>
       <c r="B20" s="50"/>
       <c r="C20" s="47"/>
     </row>
-    <row r="21" spans="1:3" s="42" customFormat="1" ht="14">
+    <row r="21" spans="1:3" s="42" customFormat="1" ht="14.25">
       <c r="A21" s="40"/>
       <c r="B21" s="51"/>
       <c r="C21" s="40"/>
     </row>
-    <row r="22" spans="1:3" s="42" customFormat="1" ht="14">
+    <row r="22" spans="1:3" s="42" customFormat="1" ht="14.25">
       <c r="A22" s="40"/>
       <c r="B22" s="51"/>
       <c r="C22" s="40"/>
     </row>
-    <row r="23" spans="1:3" s="42" customFormat="1" ht="16">
+    <row r="23" spans="1:3" s="42" customFormat="1" ht="15.75">
       <c r="A23" s="52"/>
       <c r="B23" s="53"/>
     </row>
@@ -6777,7 +6773,7 @@
       <c r="A29" s="54"/>
       <c r="B29" s="56"/>
     </row>
-    <row r="30" spans="1:3" s="42" customFormat="1" ht="14">
+    <row r="30" spans="1:3" s="42" customFormat="1" ht="14.25">
       <c r="B30" s="57"/>
     </row>
     <row r="31" spans="1:3" s="42" customFormat="1"/>
@@ -6785,8 +6781,8 @@
   </sheetData>
   <phoneticPr fontId="42" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="B14" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B14" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>